<commit_message>
Synchronized the xlsx with the CSV
</commit_message>
<xml_diff>
--- a/RDF Mapping.xlsx
+++ b/RDF Mapping.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="155">
   <si>
     <t xml:space="preserve">Label</t>
   </si>
@@ -167,7 +167,7 @@
     <t xml:space="preserve">Collection Dates</t>
   </si>
   <si>
-    <t xml:space="preserve">collectionDate</t>
+    <t xml:space="preserve">collectionDates</t>
   </si>
   <si>
     <t xml:space="preserve">Universe</t>
@@ -305,7 +305,7 @@
     <t xml:space="preserve">JEL classification</t>
   </si>
   <si>
-    <t xml:space="preserve">subject</t>
+    <t xml:space="preserve">jelClassification</t>
   </si>
   <si>
     <t xml:space="preserve">Might need to reference JEL XML explicitly</t>
@@ -366,9 +366,6 @@
   </si>
   <si>
     <t xml:space="preserve">orgName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">organization</t>
   </si>
   <si>
     <t xml:space="preserve">Grant Number</t>
@@ -624,12 +621,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -701,8 +698,8 @@
   </sheetPr>
   <dimension ref="A1:AA72"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A52" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F37" activeCellId="0" sqref="F37"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C53" activeCellId="0" sqref="C53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1263,13 +1260,13 @@
         <v>93</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="C37" s="3" t="s">
         <v>94</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="F37" s="0" t="s">
         <v>95</v>
@@ -1401,12 +1398,12 @@
         <v>97</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B53" s="3" t="s">
         <v>8</v>
@@ -1417,7 +1414,7 @@
     </row>
     <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B54" s="3" t="s">
         <v>8</v>
@@ -1438,7 +1435,7 @@
     </row>
     <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B57" s="3" t="s">
         <v>8</v>
@@ -1449,24 +1446,24 @@
     </row>
     <row r="58" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="B58" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="B58" s="3" t="s">
+      <c r="C58" s="3" t="s">
         <v>120</v>
-      </c>
-      <c r="C58" s="3" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="C59" s="3" t="s">
         <v>122</v>
-      </c>
-      <c r="B59" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="C59" s="3" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1481,7 +1478,7 @@
     </row>
     <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B62" s="3" t="s">
         <v>8</v>
@@ -1492,29 +1489,29 @@
     </row>
     <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="B63" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="B63" s="3" t="s">
+      <c r="C63" s="3" t="s">
         <v>120</v>
-      </c>
-      <c r="C63" s="3" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="C64" s="3" t="s">
         <v>122</v>
-      </c>
-      <c r="B64" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="C64" s="3" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B66" s="5"/>
       <c r="C66" s="5"/>
@@ -1556,7 +1553,7 @@
     </row>
     <row r="68" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B68" s="3" t="s">
         <v>8</v>
@@ -1577,21 +1574,21 @@
     </row>
     <row r="71" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="B71" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="B71" s="3" t="s">
+      <c r="C71" s="3" t="s">
         <v>126</v>
-      </c>
-      <c r="C71" s="3" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="B72" s="3" t="s">
         <v>128</v>
-      </c>
-      <c r="B72" s="3" t="s">
-        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -1652,7 +1649,7 @@
         <v>102</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1660,18 +1657,18 @@
         <v>102</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C4" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>132</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1679,7 +1676,7 @@
         <v>102</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1687,7 +1684,7 @@
         <v>102</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1695,7 +1692,7 @@
         <v>102</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1703,7 +1700,7 @@
         <v>102</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1711,7 +1708,7 @@
         <v>102</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1719,7 +1716,7 @@
         <v>102</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1727,7 +1724,7 @@
         <v>102</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1735,7 +1732,7 @@
         <v>102</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1743,7 +1740,7 @@
         <v>102</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1751,7 +1748,7 @@
         <v>102</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1759,7 +1756,7 @@
         <v>102</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1767,7 +1764,7 @@
         <v>102</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1775,7 +1772,7 @@
         <v>102</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1784,7 +1781,7 @@
         <v>25</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D18" s="6"/>
       <c r="E18" s="6"/>
@@ -1814,7 +1811,7 @@
         <v>25</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1822,7 +1819,7 @@
         <v>25</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1830,10 +1827,10 @@
         <v>25</v>
       </c>
       <c r="C21" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="D21" s="3" t="s">
         <v>150</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1841,7 +1838,7 @@
         <v>25</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1850,7 +1847,7 @@
         <v>25</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D23" s="6"/>
       <c r="E23" s="6"/>
@@ -1880,10 +1877,10 @@
         <v>25</v>
       </c>
       <c r="C24" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="D24" s="3" t="s">
         <v>154</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>155</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
After merge, further adjustments.
</commit_message>
<xml_diff>
--- a/RDF Mapping.xlsx
+++ b/RDF Mapping.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="160">
   <si>
     <t xml:space="preserve">Label</t>
   </si>
@@ -56,6 +56,15 @@
     <t xml:space="preserve">People</t>
   </si>
   <si>
+    <t xml:space="preserve">Actual rights holder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rightsHolder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">People/Organization</t>
+  </si>
+  <si>
     <t xml:space="preserve">ID</t>
   </si>
   <si>
@@ -113,12 +122,6 @@
     <t xml:space="preserve">publisher</t>
   </si>
   <si>
-    <t xml:space="preserve">Copyright Holder</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rightsHolder</t>
-  </si>
-  <si>
     <t xml:space="preserve">Bibliographic Citation</t>
   </si>
   <si>
@@ -287,7 +290,7 @@
     <t xml:space="preserve">Currently implemented as Seq/String</t>
   </si>
   <si>
-    <t xml:space="preserve">Original ICPSR Release</t>
+    <t xml:space="preserve">Date project was created</t>
   </si>
   <si>
     <t xml:space="preserve">created</t>
@@ -708,10 +711,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AA74"/>
+  <dimension ref="A1:AA1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
+      <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -771,7 +774,7 @@
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
     </row>
-    <row r="4" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
         <v>11</v>
       </c>
@@ -784,28 +787,27 @@
       <c r="D4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>15</v>
-      </c>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
     </row>
     <row r="5" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="F5" s="3" t="s">
         <v>18</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -819,501 +821,502 @@
         <v>20</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6" s="3"/>
+        <v>21</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>14</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="E7" s="3"/>
     </row>
     <row r="8" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="D8" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
+      <c r="E8" s="3" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>29</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
     </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
     </row>
     <row r="11" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E11" s="3"/>
       <c r="F11" s="3" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="3" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="3" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="3" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="3" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="3" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="3" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="3" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="3" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="F39" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1328,73 +1331,73 @@
     </row>
     <row r="42" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="3" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="3" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="3" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="3" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="3" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="3" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="2" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
@@ -1404,29 +1407,29 @@
     </row>
     <row r="50" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="3" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
@@ -1436,40 +1439,40 @@
     </row>
     <row r="54" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="3" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="3" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B55" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="3" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B56" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
@@ -1479,40 +1482,40 @@
     </row>
     <row r="59" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="3" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B59" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="3" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="3" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B63" s="2"/>
       <c r="C63" s="2"/>
@@ -1522,40 +1525,40 @@
     </row>
     <row r="64" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="3" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B64" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="3" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="3" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="4" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B68" s="5"/>
       <c r="C68" s="5"/>
@@ -1586,29 +1589,29 @@
     </row>
     <row r="69" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="3" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B69" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="3" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B70" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B72" s="2"/>
       <c r="C72" s="2"/>
@@ -1618,23 +1621,24 @@
     </row>
     <row r="73" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="3" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="3" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>132</v>
-      </c>
-    </row>
+        <v>133</v>
+      </c>
+    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="7">
     <mergeCell ref="A2:F2"/>
@@ -1690,142 +1694,142 @@
     </row>
     <row r="2" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="3" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="3" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="3" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="3" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="3" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="3" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="3" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="3" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="3" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="3" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="3" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="3" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="3" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="3" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="3" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="3" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="6"/>
       <c r="B18" s="7" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D18" s="6"/>
       <c r="E18" s="6"/>
@@ -1852,46 +1856,46 @@
     </row>
     <row r="19" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="3" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="3" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="3" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="3" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="6"/>
       <c r="B23" s="7" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="D23" s="6"/>
       <c r="E23" s="6"/>
@@ -1918,13 +1922,13 @@
     </row>
     <row r="24" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="3" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
   </sheetData>

</xml_diff>